<commit_message>
added data 2019 cleaning data 2019 update DOAJ API call
</commit_message>
<xml_diff>
--- a/data/gu/original_data/gu_korrigeringar_2019.xlsx
+++ b/data/gu/original_data/gu_korrigeringar_2019.xlsx
@@ -38,12 +38,6 @@
     <t>period</t>
   </si>
   <si>
-    <t>SEK</t>
-  </si>
-  <si>
-    <t>DOI</t>
-  </si>
-  <si>
     <t>is_hybrid</t>
   </si>
   <si>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>gu</t>
+  </si>
+  <si>
+    <t>sek</t>
+  </si>
+  <si>
+    <t>doi</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,36 +435,36 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>2019</v>
@@ -476,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>2019</v>
@@ -493,10 +493,10 @@
         <v>16074</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>2019</v>
@@ -513,10 +513,10 @@
         <v>13742</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>2019</v>
@@ -533,18 +533,18 @@
         <v>28750</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>2019</v>
@@ -553,18 +553,18 @@
         <v>26370</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>2019</v>
@@ -573,18 +573,18 @@
         <v>29176</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>2019</v>
@@ -593,13 +593,13 @@
         <v>21750</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>